<commit_message>
As Navigation TC creator, I closed my review side and waiting for verification.
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_NAVIGATION _REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_NAVIGATION _REVIEWS.xlsx
@@ -1,42 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\pulled repo\Group-3-Learning-hub-dev\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gehad\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700A4EEF-47FD-4036-8F7E-031976679EFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
     <sheet name="LH_TC_NAVIGATION _REVIEWS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>Author</t>
   </si>
@@ -274,11 +264,17 @@
   <si>
     <t>initial version of navigation test cases review</t>
   </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>NotApplicable</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -368,10 +364,6 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -749,6 +741,10 @@
           <color indexed="64"/>
         </horizontal>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -779,12 +775,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="4">
-    <tableColumn id="1" name="Version Number" dataDxfId="15"/>
-    <tableColumn id="2" name="Author" dataDxfId="14"/>
-    <tableColumn id="3" name="Updated Section" dataDxfId="13"/>
-    <tableColumn id="4" name="Date" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="12">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -793,18 +789,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" name="Date" dataDxfId="10"/>
-    <tableColumn id="11" name="Review ID" dataDxfId="9"/>
-    <tableColumn id="2" name="Reviewed Entity" dataDxfId="8"/>
-    <tableColumn id="3" name="Reviewer" dataDxfId="7"/>
-    <tableColumn id="4" name="Version" dataDxfId="6"/>
-    <tableColumn id="5" name="Review Comments" dataDxfId="5"/>
-    <tableColumn id="6" name="Actions" dataDxfId="4"/>
-    <tableColumn id="7" name="Owner" dataDxfId="3"/>
-    <tableColumn id="8" name="Owner Status" dataDxfId="2"/>
-    <tableColumn id="9" name="Reviewer verification" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1106,10 +1102,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1146,7 +1142,7 @@
         <v>38</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2:D9" ca="1" si="0">TODAY()</f>
+        <f t="shared" ref="D2" ca="1" si="0">TODAY()</f>
         <v>45768</v>
       </c>
     </row>
@@ -1201,11 +1197,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1281,7 +1277,7 @@
         <v>21</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>18</v>
@@ -1313,7 +1309,7 @@
         <v>21</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>18</v>
@@ -1329,8 +1325,12 @@
       <c r="C4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F4" s="7" t="s">
         <v>27</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>21</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>18</v>
@@ -1373,7 +1373,7 @@
         <v>21</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>18</v>
@@ -1405,7 +1405,7 @@
         <v>21</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>18</v>
@@ -1486,13 +1486,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v1.1 verify the status after modification
verify the status and closed after modification done on the navigation test cases
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_NAVIGATION _REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_NAVIGATION _REVIEWS.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gehad\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\pulled repo\Group-3-Learning-hub-dev\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700A4EEF-47FD-4036-8F7E-031976679EFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
     <sheet name="LH_TC_NAVIGATION _REVIEWS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>Author</t>
   </si>
@@ -81,9 +80,6 @@
   <si>
     <t>Ahmed
 Abuzaid</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t xml:space="preserve">test cases file doesn't follow main test case template </t>
@@ -270,11 +266,17 @@
   <si>
     <t>NotApplicable</t>
   </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>verify the status after modification done on the test cases</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -775,12 +777,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="12">
+    <tableColumn id="1" name="Version Number" dataDxfId="15"/>
+    <tableColumn id="2" name="Author" dataDxfId="14"/>
+    <tableColumn id="3" name="Updated Section" dataDxfId="13"/>
+    <tableColumn id="4" name="Date" dataDxfId="12">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -789,18 +791,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="11" name="Review ID" dataDxfId="8"/>
+    <tableColumn id="2" name="Reviewed Entity" dataDxfId="7"/>
+    <tableColumn id="3" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="4" name="Version" dataDxfId="5"/>
+    <tableColumn id="5" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="6" name="Actions" dataDxfId="3"/>
+    <tableColumn id="7" name="Owner" dataDxfId="2"/>
+    <tableColumn id="8" name="Owner Status" dataDxfId="1"/>
+    <tableColumn id="9" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1102,11 +1104,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,21 +1138,30 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2" ca="1" si="0">TODAY()</f>
+        <f t="shared" ref="D2:D3" ca="1" si="0">TODAY()</f>
         <v>45768</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45768</v>
+      </c>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1197,11 +1208,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A4" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1268,19 +1279,19 @@
         <v>2</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>21</v>
-      </c>
       <c r="I2" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="189" x14ac:dyDescent="0.35">
@@ -1288,10 +1299,10 @@
         <v>15</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>17</v>
@@ -1300,19 +1311,19 @@
         <v>2</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="252" x14ac:dyDescent="0.35">
@@ -1320,10 +1331,10 @@
         <v>15</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>17</v>
@@ -1332,19 +1343,19 @@
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="42" x14ac:dyDescent="0.35">
@@ -1352,10 +1363,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>17</v>
@@ -1364,19 +1375,19 @@
         <v>2</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.35">
@@ -1384,7 +1395,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>16</v>
@@ -1396,19 +1407,19 @@
         <v>2</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1486,13 +1497,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>